<commit_message>
Concurent DB access problem
</commit_message>
<xml_diff>
--- a/src/data-import/import/import_30_01_2023.xlsx
+++ b/src/data-import/import/import_30_01_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POLSL\TAI\projekt\piecyk-pol-hurt\src\data-import\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7E8000-573A-4E5D-AC94-AA9023A38FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B3B79B-1F1A-48D6-8DDC-A8C84796912D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>